<commit_message>
fix input team listing
</commit_message>
<xml_diff>
--- a/Web Application - Front End/public/assets/pandas_multiple.xlsx
+++ b/Web Application - Front End/public/assets/pandas_multiple.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Team0" sheetId="1" r:id="rId1"/>
+    <sheet name="Team1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>sdn</t>
   </si>
@@ -47,6 +48,15 @@
   </si>
   <si>
     <t>('480_Sarah Ochoa', 'sde1')</t>
+  </si>
+  <si>
+    <t>('331_John Ho', 'sde2')</t>
+  </si>
+  <si>
+    <t>('336_Mrs. Claudia Thomas', 'sde2')</t>
+  </si>
+  <si>
+    <t>('371_Michelle Kirby', 'sdn1')</t>
   </si>
 </sst>
 </file>
@@ -479,6 +489,142 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">

</xml_diff>